<commit_message>
Added support for bookmarks
</commit_message>
<xml_diff>
--- a/documents/Published/FunnelWithSource/FunnelWithSourceByMAQSoftwareChecklist.xlsx
+++ b/documents/Published/FunnelWithSource/FunnelWithSourceByMAQSoftwareChecklist.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="18528"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="19330"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Power BI\HFB\28-9-17\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\CustomVisuals\documents\Published\FunnelWithSource\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{38430F18-FB5C-47D5-B35D-93BE7916B20B}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="13635" xr2:uid="{4AB92824-63E9-41E2-A760-A81835BDCF59}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="13635" activeTab="1" xr2:uid="{4AB92824-63E9-41E2-A760-A81835BDCF59}"/>
   </bookViews>
   <sheets>
     <sheet name="BVTs" sheetId="1" r:id="rId1"/>
@@ -25,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="111" uniqueCount="89">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="115" uniqueCount="93">
   <si>
     <t>S no</t>
   </si>
@@ -374,6 +375,22 @@
   </si>
   <si>
     <t>Horizontal funnel visual should be rendered for selected category and measure columns</t>
+  </si>
+  <si>
+    <t>1. Go to View and tick the Bookmarks Pane
+2. In the visual, perform selection
+3. In the Bookmarks Pane, add a new bookmark and 'update' it
+4. Change the selections
+5. Click on the saved bookmark</t>
+  </si>
+  <si>
+    <t>Check Bookmarks feature</t>
+  </si>
+  <si>
+    <t>Bookmarks</t>
+  </si>
+  <si>
+    <t>Saved Bookmark should restore the selection state as saved</t>
   </si>
 </sst>
 </file>
@@ -497,12 +514,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="33">
+  <cellXfs count="34">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
@@ -518,12 +532,6 @@
     <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" indent="2"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -531,9 +539,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -553,6 +558,34 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -562,24 +595,11 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -895,16 +915,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BFD979CE-A2F4-4A57-BF74-C680FEBF31B0}">
-  <dimension ref="A1:E21"/>
+  <dimension ref="A1:E22"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E9" sqref="E9"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E21" sqref="E21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="4.7109375" style="10" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="20.42578125" style="10" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="4.7109375" style="7" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="20.42578125" style="7" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="72.42578125" style="1" customWidth="1"/>
     <col min="4" max="4" width="99" style="1" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="82.28515625" style="1" customWidth="1"/>
@@ -912,288 +932,304 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A1" s="11" t="s">
+      <c r="A1" s="8" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="11" t="s">
+      <c r="B1" s="8" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="12" t="s">
+      <c r="C1" s="9" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="12" t="s">
+      <c r="D1" s="9" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="12" t="s">
+      <c r="E1" s="9" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A2" s="23">
+      <c r="A2" s="29">
         <v>1</v>
       </c>
-      <c r="B2" s="23" t="s">
+      <c r="B2" s="29" t="s">
         <v>9</v>
       </c>
-      <c r="C2" s="27" t="s">
+      <c r="C2" s="21" t="s">
         <v>10</v>
       </c>
-      <c r="D2" s="16" t="s">
+      <c r="D2" s="12" t="s">
         <v>76</v>
       </c>
-      <c r="E2" s="30" t="s">
+      <c r="E2" s="24" t="s">
         <v>75</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A3" s="24"/>
-      <c r="B3" s="24"/>
-      <c r="C3" s="28"/>
-      <c r="D3" s="16" t="s">
+      <c r="A3" s="30"/>
+      <c r="B3" s="30"/>
+      <c r="C3" s="22"/>
+      <c r="D3" s="12" t="s">
         <v>77</v>
       </c>
-      <c r="E3" s="31"/>
+      <c r="E3" s="25"/>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A4" s="24"/>
-      <c r="B4" s="24"/>
-      <c r="C4" s="28"/>
-      <c r="D4" s="26" t="s">
+      <c r="A4" s="30"/>
+      <c r="B4" s="30"/>
+      <c r="C4" s="22"/>
+      <c r="D4" s="19" t="s">
         <v>78</v>
       </c>
-      <c r="E4" s="31"/>
+      <c r="E4" s="25"/>
     </row>
     <row r="5" spans="1:5" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="24"/>
-      <c r="B5" s="24"/>
-      <c r="C5" s="29"/>
-      <c r="D5" s="19" t="s">
+      <c r="A5" s="30"/>
+      <c r="B5" s="30"/>
+      <c r="C5" s="23"/>
+      <c r="D5" s="15" t="s">
         <v>79</v>
       </c>
-      <c r="E5" s="32"/>
+      <c r="E5" s="26"/>
     </row>
     <row r="6" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A6" s="24"/>
-      <c r="B6" s="24"/>
-      <c r="C6" s="19" t="s">
+      <c r="A6" s="30"/>
+      <c r="B6" s="30"/>
+      <c r="C6" s="15" t="s">
         <v>80</v>
       </c>
-      <c r="D6" s="16" t="s">
+      <c r="D6" s="12" t="s">
         <v>81</v>
       </c>
-      <c r="E6" s="16" t="s">
+      <c r="E6" s="12" t="s">
         <v>88</v>
       </c>
     </row>
     <row r="7" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A7" s="24"/>
-      <c r="B7" s="24"/>
-      <c r="C7" s="19" t="s">
+      <c r="A7" s="30"/>
+      <c r="B7" s="30"/>
+      <c r="C7" s="15" t="s">
         <v>82</v>
       </c>
-      <c r="D7" s="16" t="s">
+      <c r="D7" s="12" t="s">
         <v>83</v>
       </c>
-      <c r="E7" s="16" t="s">
+      <c r="E7" s="12" t="s">
         <v>84</v>
       </c>
     </row>
     <row r="8" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A8" s="25"/>
-      <c r="B8" s="25"/>
-      <c r="C8" s="19" t="s">
+      <c r="A8" s="31"/>
+      <c r="B8" s="31"/>
+      <c r="C8" s="15" t="s">
         <v>85</v>
       </c>
-      <c r="D8" s="19" t="s">
+      <c r="D8" s="15" t="s">
         <v>86</v>
       </c>
-      <c r="E8" s="19" t="s">
+      <c r="E8" s="15" t="s">
         <v>87</v>
       </c>
     </row>
     <row r="9" spans="1:5" ht="45" x14ac:dyDescent="0.25">
-      <c r="A9" s="17">
+      <c r="A9" s="13">
         <v>2</v>
       </c>
-      <c r="B9" s="17" t="s">
+      <c r="B9" s="13" t="s">
         <v>5</v>
       </c>
-      <c r="C9" s="14" t="s">
+      <c r="C9" s="10" t="s">
         <v>6</v>
       </c>
-      <c r="D9" s="15" t="s">
+      <c r="D9" s="11" t="s">
         <v>15</v>
       </c>
-      <c r="E9" s="14" t="s">
+      <c r="E9" s="10" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="10" spans="1:5" ht="45" x14ac:dyDescent="0.25">
-      <c r="A10" s="13">
+      <c r="A10" s="28">
         <v>3</v>
       </c>
-      <c r="B10" s="18" t="s">
+      <c r="B10" s="27" t="s">
         <v>46</v>
       </c>
-      <c r="C10" s="16" t="s">
+      <c r="C10" s="12" t="s">
         <v>68</v>
       </c>
-      <c r="D10" s="19" t="s">
+      <c r="D10" s="15" t="s">
         <v>70</v>
       </c>
-      <c r="E10" s="16" t="s">
+      <c r="E10" s="12" t="s">
         <v>71</v>
       </c>
     </row>
     <row r="11" spans="1:5" ht="60" x14ac:dyDescent="0.25">
-      <c r="A11" s="13"/>
-      <c r="B11" s="18"/>
-      <c r="C11" s="14" t="s">
+      <c r="A11" s="28"/>
+      <c r="B11" s="27"/>
+      <c r="C11" s="10" t="s">
         <v>12</v>
       </c>
-      <c r="D11" s="19" t="s">
+      <c r="D11" s="15" t="s">
         <v>72</v>
       </c>
-      <c r="E11" s="16" t="s">
+      <c r="E11" s="12" t="s">
         <v>47</v>
       </c>
     </row>
     <row r="12" spans="1:5" ht="45" x14ac:dyDescent="0.25">
-      <c r="A12" s="13">
+      <c r="A12" s="28">
         <v>4</v>
       </c>
-      <c r="B12" s="18" t="s">
+      <c r="B12" s="27" t="s">
         <v>48</v>
       </c>
-      <c r="C12" s="16" t="s">
+      <c r="C12" s="12" t="s">
         <v>69</v>
       </c>
-      <c r="D12" s="19" t="s">
+      <c r="D12" s="15" t="s">
         <v>73</v>
       </c>
-      <c r="E12" s="14" t="s">
+      <c r="E12" s="10" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="13" spans="1:5" ht="60" x14ac:dyDescent="0.25">
-      <c r="A13" s="13"/>
-      <c r="B13" s="18"/>
-      <c r="C13" s="14" t="s">
+      <c r="A13" s="28"/>
+      <c r="B13" s="27"/>
+      <c r="C13" s="10" t="s">
         <v>12</v>
       </c>
-      <c r="D13" s="19" t="s">
+      <c r="D13" s="15" t="s">
         <v>74</v>
       </c>
-      <c r="E13" s="16" t="s">
+      <c r="E13" s="12" t="s">
         <v>47</v>
       </c>
     </row>
     <row r="14" spans="1:5" ht="45" x14ac:dyDescent="0.25">
-      <c r="A14" s="13">
+      <c r="A14" s="28">
         <v>5</v>
       </c>
-      <c r="B14" s="18" t="s">
+      <c r="B14" s="27" t="s">
         <v>49</v>
       </c>
-      <c r="C14" s="16" t="s">
+      <c r="C14" s="12" t="s">
         <v>50</v>
       </c>
-      <c r="D14" s="19" t="s">
+      <c r="D14" s="15" t="s">
         <v>51</v>
       </c>
-      <c r="E14" s="16" t="s">
+      <c r="E14" s="12" t="s">
         <v>52</v>
       </c>
     </row>
     <row r="15" spans="1:5" ht="45" x14ac:dyDescent="0.25">
-      <c r="A15" s="13"/>
-      <c r="B15" s="18"/>
-      <c r="C15" s="16" t="s">
+      <c r="A15" s="28"/>
+      <c r="B15" s="27"/>
+      <c r="C15" s="12" t="s">
         <v>53</v>
       </c>
-      <c r="D15" s="19" t="s">
+      <c r="D15" s="15" t="s">
         <v>54</v>
       </c>
-      <c r="E15" s="16" t="s">
+      <c r="E15" s="12" t="s">
         <v>55</v>
       </c>
     </row>
     <row r="16" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A16" s="13">
+      <c r="A16" s="28">
         <v>6</v>
       </c>
-      <c r="B16" s="18" t="s">
+      <c r="B16" s="27" t="s">
         <v>56</v>
       </c>
-      <c r="C16" s="16" t="s">
+      <c r="C16" s="12" t="s">
         <v>59</v>
       </c>
-      <c r="D16" s="19" t="s">
+      <c r="D16" s="15" t="s">
         <v>57</v>
       </c>
-      <c r="E16" s="19" t="s">
+      <c r="E16" s="15" t="s">
         <v>58</v>
       </c>
     </row>
     <row r="17" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A17" s="13"/>
-      <c r="B17" s="18"/>
-      <c r="C17" s="16" t="s">
+      <c r="A17" s="28"/>
+      <c r="B17" s="27"/>
+      <c r="C17" s="12" t="s">
         <v>60</v>
       </c>
-      <c r="D17" s="19" t="s">
+      <c r="D17" s="15" t="s">
         <v>61</v>
       </c>
-      <c r="E17" s="19" t="s">
+      <c r="E17" s="15" t="s">
         <v>58</v>
       </c>
     </row>
     <row r="18" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A18" s="13"/>
-      <c r="B18" s="18"/>
-      <c r="C18" s="16" t="s">
+      <c r="A18" s="28"/>
+      <c r="B18" s="27"/>
+      <c r="C18" s="12" t="s">
         <v>62</v>
       </c>
-      <c r="D18" s="19" t="s">
+      <c r="D18" s="15" t="s">
         <v>63</v>
       </c>
-      <c r="E18" s="19" t="s">
+      <c r="E18" s="15" t="s">
         <v>58</v>
       </c>
     </row>
     <row r="19" spans="1:5" ht="45" x14ac:dyDescent="0.25">
-      <c r="A19" s="13">
+      <c r="A19" s="28">
         <v>7</v>
       </c>
-      <c r="B19" s="18" t="s">
+      <c r="B19" s="27" t="s">
         <v>64</v>
       </c>
-      <c r="C19" s="14" t="s">
+      <c r="C19" s="10" t="s">
         <v>13</v>
       </c>
-      <c r="D19" s="19" t="s">
+      <c r="D19" s="15" t="s">
         <v>65</v>
       </c>
-      <c r="E19" s="14" t="s">
+      <c r="E19" s="10" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="20" spans="1:5" ht="45" x14ac:dyDescent="0.25">
-      <c r="A20" s="13"/>
-      <c r="B20" s="18"/>
-      <c r="C20" s="20" t="s">
+      <c r="A20" s="28"/>
+      <c r="B20" s="27"/>
+      <c r="C20" s="16" t="s">
         <v>8</v>
       </c>
-      <c r="D20" s="21" t="s">
+      <c r="D20" s="17" t="s">
         <v>66</v>
       </c>
-      <c r="E20" s="22" t="s">
+      <c r="E20" s="18" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="D21" s="2"/>
-      <c r="E21" s="2"/>
+    <row r="21" spans="1:5" ht="75" x14ac:dyDescent="0.25">
+      <c r="A21" s="13">
+        <v>8</v>
+      </c>
+      <c r="B21" s="14" t="s">
+        <v>91</v>
+      </c>
+      <c r="C21" s="18" t="s">
+        <v>90</v>
+      </c>
+      <c r="D21" s="15" t="s">
+        <v>89</v>
+      </c>
+      <c r="E21" s="15" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="D22" s="20"/>
     </row>
   </sheetData>
   <mergeCells count="14">
@@ -1221,8 +1257,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B9445F79-59A8-4539-BCC2-AC7C1C772DD6}">
   <dimension ref="A1:C27"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G21" sqref="G21"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E5" sqref="E5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1232,273 +1268,273 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A1" s="3" t="s">
+      <c r="A1" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="B1" s="3" t="s">
+      <c r="B1" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="C1" s="3" t="s">
+      <c r="C1" s="2" t="s">
         <v>18</v>
       </c>
     </row>
     <row r="2" spans="1:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="A2" s="4">
+      <c r="A2" s="3">
         <v>1</v>
       </c>
-      <c r="B2" s="5" t="s">
+      <c r="B2" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="C2" s="5" t="s">
+      <c r="C2" s="4" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A3" s="4">
+      <c r="A3" s="3">
         <v>2</v>
       </c>
-      <c r="B3" s="5" t="s">
+      <c r="B3" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="C3" s="5" t="s">
+      <c r="C3" s="4" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A4" s="4">
+      <c r="A4" s="3">
         <v>3</v>
       </c>
-      <c r="B4" s="5" t="s">
+      <c r="B4" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="C4" s="5" t="s">
+      <c r="C4" s="4" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A5" s="4">
+      <c r="A5" s="3">
         <v>4</v>
       </c>
-      <c r="B5" s="5" t="s">
+      <c r="B5" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="C5" s="5" t="s">
+      <c r="C5" s="4" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="6" spans="1:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="A6" s="4">
+      <c r="A6" s="3">
         <v>5</v>
       </c>
-      <c r="B6" s="5" t="s">
+      <c r="B6" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="C6" s="5" t="s">
+      <c r="C6" s="4" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="7" spans="1:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="A7" s="4">
+      <c r="A7" s="3">
         <v>6</v>
       </c>
-      <c r="B7" s="5" t="s">
+      <c r="B7" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="C7" s="5" t="s">
+      <c r="C7" s="4" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="8" spans="1:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="A8" s="4">
+      <c r="A8" s="3">
         <v>7</v>
       </c>
-      <c r="B8" s="5" t="s">
+      <c r="B8" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="C8" s="5" t="s">
+      <c r="C8" s="4" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A9" s="4">
+      <c r="A9" s="3">
         <v>8</v>
       </c>
-      <c r="B9" s="5" t="s">
+      <c r="B9" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="C9" s="5" t="s">
+      <c r="C9" s="4" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A10" s="4">
+      <c r="A10" s="3">
         <v>9</v>
       </c>
-      <c r="B10" s="5" t="s">
+      <c r="B10" s="4" t="s">
         <v>29</v>
       </c>
-      <c r="C10" s="5" t="s">
+      <c r="C10" s="4" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A11" s="4">
+      <c r="A11" s="3">
         <v>10</v>
       </c>
-      <c r="B11" s="5" t="s">
+      <c r="B11" s="4" t="s">
         <v>30</v>
       </c>
-      <c r="C11" s="5" t="s">
+      <c r="C11" s="4" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A12" s="4">
+      <c r="A12" s="3">
         <v>11</v>
       </c>
-      <c r="B12" s="5" t="s">
+      <c r="B12" s="4" t="s">
         <v>31</v>
       </c>
-      <c r="C12" s="5" t="s">
+      <c r="C12" s="4" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A13" s="4">
+      <c r="A13" s="3">
         <v>12</v>
       </c>
-      <c r="B13" s="5" t="s">
+      <c r="B13" s="4" t="s">
         <v>32</v>
       </c>
-      <c r="C13" s="5" t="s">
+      <c r="C13" s="4" t="s">
         <v>27</v>
       </c>
     </row>
     <row r="14" spans="1:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="A14" s="4">
+      <c r="A14" s="3">
         <v>13</v>
       </c>
-      <c r="B14" s="5" t="s">
+      <c r="B14" s="4" t="s">
         <v>33</v>
       </c>
-      <c r="C14" s="5" t="s">
-        <v>20</v>
+      <c r="C14" s="4" t="s">
+        <v>27</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A15" s="4">
+      <c r="A15" s="3">
         <v>14</v>
       </c>
-      <c r="B15" s="5" t="s">
+      <c r="B15" s="4" t="s">
         <v>34</v>
       </c>
-      <c r="C15" s="5" t="s">
+      <c r="C15" s="4" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A16" s="4">
+      <c r="A16" s="3">
         <v>15</v>
       </c>
-      <c r="B16" s="5" t="s">
+      <c r="B16" s="4" t="s">
         <v>35</v>
       </c>
-      <c r="C16" s="5" t="s">
+      <c r="C16" s="4" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A17" s="8">
+      <c r="A17" s="32">
         <v>16</v>
       </c>
-      <c r="B17" s="6" t="s">
+      <c r="B17" s="5" t="s">
         <v>36</v>
       </c>
-      <c r="C17" s="9" t="s">
+      <c r="C17" s="33" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A18" s="8"/>
-      <c r="B18" s="7" t="s">
+      <c r="A18" s="32"/>
+      <c r="B18" s="6" t="s">
         <v>37</v>
       </c>
-      <c r="C18" s="9"/>
+      <c r="C18" s="33"/>
     </row>
     <row r="19" spans="1:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="A19" s="8"/>
-      <c r="B19" s="7" t="s">
+      <c r="A19" s="32"/>
+      <c r="B19" s="6" t="s">
         <v>38</v>
       </c>
-      <c r="C19" s="9"/>
+      <c r="C19" s="33"/>
     </row>
     <row r="20" spans="1:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="A20" s="4">
+      <c r="A20" s="3">
         <v>17</v>
       </c>
-      <c r="B20" s="5" t="s">
+      <c r="B20" s="4" t="s">
         <v>39</v>
       </c>
-      <c r="C20" s="5" t="s">
+      <c r="C20" s="4" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A21" s="8">
+      <c r="A21" s="32">
         <v>18</v>
       </c>
-      <c r="B21" s="5" t="s">
+      <c r="B21" s="4" t="s">
         <v>40</v>
       </c>
-      <c r="C21" s="9" t="s">
+      <c r="C21" s="33" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A22" s="8"/>
-      <c r="B22" s="5" t="s">
+      <c r="A22" s="32"/>
+      <c r="B22" s="4" t="s">
         <v>41</v>
       </c>
-      <c r="C22" s="9"/>
+      <c r="C22" s="33"/>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A23" s="8"/>
-      <c r="B23" s="5" t="s">
+      <c r="A23" s="32"/>
+      <c r="B23" s="4" t="s">
         <v>42</v>
       </c>
-      <c r="C23" s="9"/>
+      <c r="C23" s="33"/>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A24" s="8"/>
-      <c r="B24" s="5"/>
-      <c r="C24" s="9"/>
+      <c r="A24" s="32"/>
+      <c r="B24" s="4"/>
+      <c r="C24" s="33"/>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A25" s="8"/>
-      <c r="B25" s="5" t="s">
+      <c r="A25" s="32"/>
+      <c r="B25" s="4" t="s">
         <v>43</v>
       </c>
-      <c r="C25" s="9"/>
+      <c r="C25" s="33"/>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A26" s="4">
+      <c r="A26" s="3">
         <v>19</v>
       </c>
-      <c r="B26" s="5" t="s">
+      <c r="B26" s="4" t="s">
         <v>44</v>
       </c>
-      <c r="C26" s="5" t="s">
+      <c r="C26" s="4" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A27" s="4">
-        <v>20</v>
-      </c>
-      <c r="B27" s="5" t="s">
+      <c r="A27" s="3">
+        <v>20</v>
+      </c>
+      <c r="B27" s="4" t="s">
         <v>45</v>
       </c>
-      <c r="C27" s="5" t="s">
+      <c r="C27" s="4" t="s">
         <v>27</v>
       </c>
     </row>

</xml_diff>